<commit_message>
brand completo y funcional
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>perro</t>
+  </si>
+  <si>
+    <t>emo</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -456,14 +459,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="0">
         <v>2</v>
@@ -486,6 +481,22 @@
       </c>
       <c r="B6" t="s" s="0">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funciona todo menos categoria
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t>emo</t>
+  </si>
+  <si>
+    <t>pedro</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t>jose</t>
+  </si>
+  <si>
+    <t>5552</t>
+  </si>
+  <si>
+    <t>dgg</t>
+  </si>
+  <si>
+    <t>fertilizante</t>
+  </si>
+  <si>
+    <t>pesticida</t>
+  </si>
+  <si>
+    <t>para pesticid</t>
   </si>
 </sst>
 </file>
@@ -443,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -483,22 +507,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -506,7 +514,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -526,6 +534,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -533,7 +555,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -548,6 +570,17 @@
       </c>
       <c r="C1" t="s" s="0">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dialoj en todo menos producto
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -45,6 +45,27 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>rfgrgfrg</t>
+  </si>
+  <si>
+    <t>cfndfh</t>
+  </si>
+  <si>
+    <t>dwdefge</t>
+  </si>
+  <si>
+    <t>sdgsdg</t>
+  </si>
+  <si>
+    <t>juan tirado</t>
+  </si>
+  <si>
+    <t>76523458</t>
+  </si>
+  <si>
+    <t>jdkdjd</t>
   </si>
 </sst>
 </file>
@@ -89,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -103,6 +124,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -110,7 +147,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -130,6 +167,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -137,7 +188,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -154,6 +205,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
combobox de producto completado
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -66,6 +66,36 @@
   </si>
   <si>
     <t>jdkdjd</t>
+  </si>
+  <si>
+    <t>cvcv</t>
+  </si>
+  <si>
+    <t>Categoría 2</t>
+  </si>
+  <si>
+    <t>Marca B</t>
+  </si>
+  <si>
+    <t>cvnn</t>
+  </si>
+  <si>
+    <t>dfnh</t>
+  </si>
+  <si>
+    <t>Categoría 1</t>
+  </si>
+  <si>
+    <t>Marca A</t>
+  </si>
+  <si>
+    <t>dfn</t>
+  </si>
+  <si>
+    <t>ssdgg</t>
+  </si>
+  <si>
+    <t>fgj</t>
   </si>
 </sst>
 </file>
@@ -223,7 +253,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -252,6 +282,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
combobox de producto completado en todos las tablas
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>fgj</t>
+  </si>
+  <si>
+    <t>dfbdfb</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -140,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -170,6 +179,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -177,7 +202,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -209,6 +234,20 @@
       </c>
       <c r="D2" t="s" s="0">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
estilos agregados a la funcionalidad
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>yuyuy</t>
+  </si>
+  <si>
+    <t>sff</t>
+  </si>
+  <si>
+    <t>df</t>
   </si>
 </sst>
 </file>
@@ -149,7 +158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -193,6 +202,14 @@
       </c>
       <c r="B5" t="s" s="0">
         <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -279,7 +296,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>13</v>
@@ -292,7 +309,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -344,6 +361,29 @@
         <v>26</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>